<commit_message>
Update to various cleanup actions
Particularly improved URLs fixing and removal of problematic ones.
Also, fixed a problem with a translation due to missing escape characters.
</commit_message>
<xml_diff>
--- a/biogeography_italian_translation.xlsx
+++ b/biogeography_italian_translation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documenti\Dottorato\Analisi statistica\GitHub\GdL_Biodiv_survey_postprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A53109-DD42-4AEB-A9E6-B21B69685F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FC5999-80FB-458D-9F1F-6691D4063E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11484" yWindow="2616" windowWidth="11484" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,12 +45,6 @@
     <t>Marina</t>
   </si>
   <si>
-    <t>Global scale (marine or terrestrial)</t>
-  </si>
-  <si>
-    <t>Globale (marina o terrestre)</t>
-  </si>
-  <si>
     <t>Nearctic</t>
   </si>
   <si>
@@ -66,9 +60,6 @@
     <t>Paleartica</t>
   </si>
   <si>
-    <t>Palearctic</t>
-  </si>
-  <si>
     <t>Afrotropical</t>
   </si>
   <si>
@@ -115,6 +106,15 @@
   </si>
   <si>
     <t>Artica</t>
+  </si>
+  <si>
+    <t>Palaearctic</t>
+  </si>
+  <si>
+    <t>Global scale \(marine or terrestrial\)</t>
+  </si>
+  <si>
+    <t>Globale \(marina o terrestre\)</t>
   </si>
 </sst>
 </file>
@@ -432,15 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,15 +448,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -464,7 +464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -472,95 +472,94 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>